<commit_message>
coloring the `extra_listdo.xlsx` rows
</commit_message>
<xml_diff>
--- a/extra_listdo.xlsx
+++ b/extra_listdo.xlsx
@@ -953,12 +953,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -995,7 +1001,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1010,6 +1016,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1045,11 +1063,11 @@
   </sheetPr>
   <dimension ref="A1:F146"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F147" activeCellId="0" sqref="F147"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.01953125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.03125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.55"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.01"/>
@@ -1080,22 +1098,22 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="n">
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="n">
         <v>2002</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1340,22 +1358,22 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="1" t="n">
+      <c r="D15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="5" t="n">
         <v>2008</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1640,22 +1658,22 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="1" t="n">
+      <c r="D30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="5" t="n">
         <v>1936</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" s="4" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2440,22 +2458,22 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
+      <c r="A70" s="4" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="B70" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E70" s="1" t="n">
+      <c r="D70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="5" t="n">
         <v>2005</v>
       </c>
-      <c r="F70" s="0" t="s">
+      <c r="F70" s="4" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2600,22 +2618,22 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="n">
+      <c r="A78" s="4" t="n">
         <v>77</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="1" t="s">
+      <c r="B78" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E78" s="1" t="n">
+      <c r="D78" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" s="5" t="n">
         <v>1964</v>
       </c>
-      <c r="F78" s="0" t="s">
+      <c r="F78" s="4" t="s">
         <v>163</v>
       </c>
     </row>
@@ -3040,22 +3058,22 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="n">
+      <c r="A100" s="4" t="n">
         <v>99</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="1" t="s">
+      <c r="B100" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E100" s="1" t="n">
+      <c r="D100" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="5" t="n">
         <v>1901</v>
       </c>
-      <c r="F100" s="0" t="s">
+      <c r="F100" s="4" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3940,42 +3958,42 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="n">
+      <c r="A145" s="4" t="n">
         <v>144</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C145" s="1" t="s">
+      <c r="B145" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="D145" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E145" s="1" t="n">
+      <c r="D145" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E145" s="5" t="n">
         <v>2007</v>
       </c>
-      <c r="F145" s="0" t="s">
+      <c r="F145" s="4" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="n">
+    <row r="146" s="6" customFormat="true" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="4" t="n">
         <v>145</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C146" s="1" t="s">
+      <c r="B146" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="D146" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E146" s="1" t="n">
+      <c r="D146" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E146" s="5" t="n">
         <v>2007</v>
       </c>
-      <c r="F146" s="0" t="s">
+      <c r="F146" s="4" t="s">
         <v>299</v>
       </c>
     </row>

</xml_diff>